<commit_message>
updates a lot of them
</commit_message>
<xml_diff>
--- a/ipa_1_2/myUtils/features.xlsx
+++ b/ipa_1_2/myUtils/features.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24228"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\stavw\Documents\GitHub\WebExperiment\ipa_1_2\myUtils\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tomer\Documents\GitHub\WebExperiment\ipa_1_2\myUtils\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34011CA7-1150-4185-94E4-ACC89865C0C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C424B461-74AB-49CC-88EF-FA3DB69BA668}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1365" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="49">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="54">
   <si>
     <t>feature</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Political Affiliation</t>
   </si>
   <si>
-    <t>question</t>
-  </si>
-  <si>
     <t>מה ההעדפה הפוליטית שלך</t>
   </si>
   <si>
@@ -172,6 +169,24 @@
   </si>
   <si>
     <t>xl-c2</t>
+  </si>
+  <si>
+    <t>question_heb</t>
+  </si>
+  <si>
+    <t>מה ההעדפה הפוליטית של {}</t>
+  </si>
+  <si>
+    <t>איפה מתרחשים התחביבים של {}</t>
+  </si>
+  <si>
+    <t>מה מבנה הגוף של {}</t>
+  </si>
+  <si>
+    <t>מה רמת האינטליגנציה של {}</t>
+  </si>
+  <si>
+    <t>question_heb_max_min_ideal</t>
   </si>
 </sst>
 </file>
@@ -182,7 +197,7 @@
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -190,7 +205,7 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -498,24 +513,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6:D10"/>
+      <selection activeCell="G1" sqref="G1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="19.25" customWidth="1"/>
-    <col min="3" max="3" width="16.75" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="8.625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="10.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="26" bestFit="1" customWidth="1"/>
+    <col min="1" max="2" width="19.28515625" customWidth="1"/>
+    <col min="3" max="3" width="16.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10.140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="26" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -530,187 +545,217 @@
         <v>2</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+        <v>48</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
         <v>4</v>
       </c>
       <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>8</v>
+      </c>
+      <c r="E2" t="s">
         <v>7</v>
       </c>
-      <c r="D2" t="s">
+      <c r="F2" t="s">
+        <v>5</v>
+      </c>
+      <c r="G2" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B3" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>8</v>
-      </c>
-      <c r="F2" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="C3" t="s">
+        <v>12</v>
+      </c>
+      <c r="D3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E3" t="s">
+        <v>16</v>
+      </c>
+      <c r="F3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G3" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>13</v>
+      </c>
+      <c r="D4" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
+        <v>20</v>
+      </c>
+      <c r="G4" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" t="s">
+        <v>11</v>
+      </c>
+      <c r="C5" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" t="s">
+        <v>23</v>
+      </c>
+      <c r="G5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
         <v>26</v>
       </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="B6" t="s">
+        <v>27</v>
+      </c>
+      <c r="C6" t="s">
+        <v>33</v>
+      </c>
+      <c r="D6" t="s">
+        <v>43</v>
+      </c>
+      <c r="E6" t="s">
+        <v>38</v>
+      </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
+      <c r="G6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
         <v>26</v>
       </c>
-      <c r="B4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F4" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+      <c r="B7" t="s">
+        <v>28</v>
+      </c>
+      <c r="C7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D7" t="s">
+        <v>44</v>
+      </c>
+      <c r="E7" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" t="s">
+        <v>34</v>
+      </c>
+      <c r="G7" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
         <v>26</v>
       </c>
-      <c r="B5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" t="s">
-        <v>15</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
-      </c>
-      <c r="F5" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>27</v>
-      </c>
-      <c r="B6" t="s">
-        <v>28</v>
-      </c>
-      <c r="C6" t="s">
-        <v>34</v>
-      </c>
-      <c r="D6" t="s">
-        <v>44</v>
-      </c>
-      <c r="E6" t="s">
-        <v>39</v>
-      </c>
-      <c r="F6" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>27</v>
-      </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
         <v>29</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>35</v>
       </c>
-      <c r="D7" t="s">
+      <c r="D8" t="s">
         <v>45</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E8" t="s">
         <v>40</v>
       </c>
-      <c r="F7" t="s">
+      <c r="F8" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>27</v>
-      </c>
-      <c r="B8" t="s">
+      <c r="G8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
         <v>30</v>
       </c>
-      <c r="C8" t="s">
+      <c r="B9" t="s">
+        <v>32</v>
+      </c>
+      <c r="C9" t="s">
         <v>36</v>
       </c>
-      <c r="D8" t="s">
+      <c r="D9" t="s">
         <v>46</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E9" t="s">
         <v>41</v>
       </c>
-      <c r="F8" t="s">
+      <c r="F9" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+      <c r="G9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" t="s">
         <v>31</v>
       </c>
-      <c r="B9" t="s">
-        <v>33</v>
-      </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>37</v>
       </c>
-      <c r="D9" t="s">
+      <c r="D10" t="s">
         <v>47</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E10" t="s">
         <v>42</v>
       </c>
-      <c r="F9" t="s">
+      <c r="F10" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
-        <v>31</v>
-      </c>
-      <c r="B10" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" t="s">
-        <v>38</v>
-      </c>
-      <c r="D10" t="s">
-        <v>48</v>
-      </c>
-      <c r="E10" t="s">
-        <v>43</v>
-      </c>
-      <c r="F10" t="s">
-        <v>38</v>
+      <c r="G10" t="s">
+        <v>37</v>
       </c>
     </row>
   </sheetData>

</xml_diff>